<commit_message>
Fix permission role RBAC yang kelewat
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/general/employee_upload_bdk.xlsx
+++ b/file/template/pusdiklat/general/employee_upload_bdk.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>DATA PEGAWAI</t>
   </si>
@@ -53,7 +53,7 @@
     <t>199910102010121004</t>
   </si>
   <si>
-    <t>Matusalkh</t>
+    <t>Johny Depp</t>
   </si>
   <si>
     <t>1200010002</t>
@@ -65,13 +65,19 @@
     <t>199910102010122004</t>
   </si>
   <si>
-    <t>Elizabeth</t>
+    <t>Sabina Altynbekova</t>
   </si>
   <si>
     <t>1200010101</t>
   </si>
   <si>
     <t>Subbagian Tata Usaha Dan Kepatuhan Internal</t>
+  </si>
+  <si>
+    <t>199910112010121004</t>
+  </si>
+  <si>
+    <t>Robert Pattinson</t>
   </si>
   <si>
     <t>1200010200</t>
@@ -120,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,13 +142,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -168,6 +168,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -298,7 +305,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,31 +315,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,31 +355,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,15 +391,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,7 +427,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -493,7 +500,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -585,11 +592,11 @@
         <v>12</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="15" t="str">
         <f aca="false">VLOOKUP(D4,$J$23:$K$26,2)</f>
-        <v>PRANATA KOMPUTER</v>
+        <v>PELAKSANA</v>
       </c>
       <c r="F4" s="16" t="n">
         <v>345</v>
@@ -623,11 +630,11 @@
         <v>16</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="15" t="str">
         <f aca="false">VLOOKUP(D5,$J$23:$K$26,2)</f>
-        <v>PRANATA KOMPUTER</v>
+        <v>PELAKSANA</v>
       </c>
       <c r="F5" s="16" t="n">
         <v>346</v>
@@ -654,30 +661,38 @@
       <c r="A6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15" t="e">
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15" t="str">
         <f aca="false">VLOOKUP(D6,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17" t="e">
+        <v>PELAKSANA</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>347</v>
+      </c>
+      <c r="G6" s="17" t="str">
         <f aca="false">VLOOKUP(F6,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H6" s="17" t="e">
+        <v>1200010300</v>
+      </c>
+      <c r="H6" s="17" t="str">
         <f aca="false">VLOOKUP(F6,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <v>Seksi Evaluasi Dan Informasi</v>
       </c>
       <c r="J6" s="18" t="n">
         <v>346</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,27 +702,33 @@
       <c r="B7" s="16"/>
       <c r="C7" s="20"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="15" t="e">
+      <c r="E7" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D7,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F7" s="16"/>
-      <c r="G7" s="17" t="e">
+      <c r="G7" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F7,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H7" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H7" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F7,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J7" s="18" t="n">
         <v>347</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,18 +738,24 @@
       <c r="B8" s="16"/>
       <c r="C8" s="20"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="15" t="e">
+      <c r="E8" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D8,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="17" t="e">
+      <c r="G8" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F8,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H8" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F8,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,18 +765,24 @@
       <c r="B9" s="16"/>
       <c r="C9" s="20"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="15" t="e">
+      <c r="E9" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D9,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="17" t="e">
+      <c r="G9" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F9,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H9" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H9" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F9,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,18 +792,24 @@
       <c r="B10" s="16"/>
       <c r="C10" s="20"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="15" t="e">
+      <c r="E10" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D10,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F10" s="16"/>
-      <c r="G10" s="17" t="e">
+      <c r="G10" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F10,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H10" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H10" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F10,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,18 +819,24 @@
       <c r="B11" s="16"/>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="15" t="e">
+      <c r="E11" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D11,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F11" s="16"/>
-      <c r="G11" s="17" t="e">
+      <c r="G11" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F11,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H11" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H11" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F11,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,18 +846,24 @@
       <c r="B12" s="16"/>
       <c r="C12" s="20"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="15" t="e">
+      <c r="E12" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D12,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F12" s="16"/>
-      <c r="G12" s="17" t="e">
+      <c r="G12" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F12,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H12" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H12" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F12,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,18 +873,24 @@
       <c r="B13" s="16"/>
       <c r="C13" s="20"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="15" t="e">
+      <c r="E13" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D13,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F13" s="16"/>
-      <c r="G13" s="17" t="e">
+      <c r="G13" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F13,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H13" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H13" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F13,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,18 +900,24 @@
       <c r="B14" s="16"/>
       <c r="C14" s="20"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="15" t="e">
+      <c r="E14" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D14,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F14" s="16"/>
-      <c r="G14" s="17" t="e">
+      <c r="G14" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F14,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H14" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F14,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,18 +927,24 @@
       <c r="B15" s="16"/>
       <c r="C15" s="20"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="15" t="e">
+      <c r="E15" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D15,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F15" s="16"/>
-      <c r="G15" s="17" t="e">
+      <c r="G15" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F15,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H15" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H15" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F15,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,18 +954,24 @@
       <c r="B16" s="16"/>
       <c r="C16" s="20"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="15" t="e">
+      <c r="E16" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D16,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F16" s="16"/>
-      <c r="G16" s="17" t="e">
+      <c r="G16" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F16,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H16" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H16" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F16,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,18 +981,24 @@
       <c r="B17" s="16"/>
       <c r="C17" s="20"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="15" t="e">
+      <c r="E17" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D17,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F17" s="16"/>
-      <c r="G17" s="17" t="e">
+      <c r="G17" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F17,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H17" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H17" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F17,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,18 +1008,24 @@
       <c r="B18" s="16"/>
       <c r="C18" s="20"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="15" t="e">
+      <c r="E18" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D18,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F18" s="16"/>
-      <c r="G18" s="17" t="e">
+      <c r="G18" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F18,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H18" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H18" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F18,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,18 +1035,24 @@
       <c r="B19" s="16"/>
       <c r="C19" s="20"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="15" t="e">
+      <c r="E19" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D19,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="17" t="e">
+      <c r="G19" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F19,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H19" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H19" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F19,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,18 +1062,24 @@
       <c r="B20" s="16"/>
       <c r="C20" s="20"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="15" t="e">
+      <c r="E20" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D20,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F20" s="16"/>
-      <c r="G20" s="17" t="e">
+      <c r="G20" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F20,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H20" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H20" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F20,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,18 +1089,24 @@
       <c r="B21" s="16"/>
       <c r="C21" s="20"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="15" t="e">
+      <c r="E21" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D21,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="17" t="e">
+      <c r="G21" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F21,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H21" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H21" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F21,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,24 +1116,30 @@
       <c r="B22" s="16"/>
       <c r="C22" s="20"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="15" t="e">
+      <c r="E22" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D22,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F22" s="16"/>
-      <c r="G22" s="17" t="e">
+      <c r="G22" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F22,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H22" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F22,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J22" s="21" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,24 +1149,30 @@
       <c r="B23" s="16"/>
       <c r="C23" s="20"/>
       <c r="D23" s="14"/>
-      <c r="E23" s="15" t="e">
+      <c r="E23" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D23,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F23" s="16"/>
-      <c r="G23" s="17" t="e">
+      <c r="G23" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F23,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H23" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H23" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F23,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J23" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,24 +1182,30 @@
       <c r="B24" s="16"/>
       <c r="C24" s="20"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="15" t="e">
+      <c r="E24" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D24,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F24" s="16"/>
-      <c r="G24" s="17" t="e">
+      <c r="G24" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F24,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H24" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H24" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F24,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J24" s="21" t="n">
         <v>2</v>
       </c>
       <c r="K24" s="22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,24 +1215,30 @@
       <c r="B25" s="16"/>
       <c r="C25" s="20"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="15" t="e">
+      <c r="E25" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D25,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F25" s="16"/>
-      <c r="G25" s="17" t="e">
+      <c r="G25" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F25,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H25" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H25" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F25,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J25" s="21" t="n">
         <v>3</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,24 +1248,30 @@
       <c r="B26" s="16"/>
       <c r="C26" s="20"/>
       <c r="D26" s="14"/>
-      <c r="E26" s="15" t="e">
+      <c r="E26" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D26,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F26" s="16"/>
-      <c r="G26" s="17" t="e">
+      <c r="G26" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F26,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H26" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H26" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F26,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="J26" s="21" t="n">
         <v>4</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,18 +1281,24 @@
       <c r="B27" s="16"/>
       <c r="C27" s="20"/>
       <c r="D27" s="14"/>
-      <c r="E27" s="15" t="e">
+      <c r="E27" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D27,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F27" s="16"/>
-      <c r="G27" s="17" t="e">
+      <c r="G27" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F27,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H27" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H27" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F27,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,18 +1308,24 @@
       <c r="B28" s="16"/>
       <c r="C28" s="20"/>
       <c r="D28" s="14"/>
-      <c r="E28" s="15" t="e">
+      <c r="E28" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D28,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F28" s="16"/>
-      <c r="G28" s="17" t="e">
+      <c r="G28" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F28,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H28" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H28" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F28,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,18 +1335,24 @@
       <c r="B29" s="16"/>
       <c r="C29" s="20"/>
       <c r="D29" s="14"/>
-      <c r="E29" s="15" t="e">
+      <c r="E29" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D29,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="17" t="e">
+      <c r="G29" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F29,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H29" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H29" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F29,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,18 +1362,24 @@
       <c r="B30" s="16"/>
       <c r="C30" s="20"/>
       <c r="D30" s="14"/>
-      <c r="E30" s="15" t="e">
+      <c r="E30" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D30,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F30" s="16"/>
-      <c r="G30" s="17" t="e">
+      <c r="G30" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F30,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H30" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H30" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F30,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,18 +1389,24 @@
       <c r="B31" s="16"/>
       <c r="C31" s="20"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="15" t="e">
+      <c r="E31" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D31,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F31" s="16"/>
-      <c r="G31" s="17" t="e">
+      <c r="G31" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F31,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H31" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H31" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F31,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,18 +1416,24 @@
       <c r="B32" s="16"/>
       <c r="C32" s="20"/>
       <c r="D32" s="14"/>
-      <c r="E32" s="15" t="e">
+      <c r="E32" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D32,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F32" s="16"/>
-      <c r="G32" s="17" t="e">
+      <c r="G32" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F32,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H32" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H32" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F32,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,18 +1443,24 @@
       <c r="B33" s="16"/>
       <c r="C33" s="20"/>
       <c r="D33" s="14"/>
-      <c r="E33" s="15" t="e">
+      <c r="E33" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D33,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F33" s="16"/>
-      <c r="G33" s="17" t="e">
+      <c r="G33" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F33,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H33" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H33" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F33,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,18 +1470,24 @@
       <c r="B34" s="16"/>
       <c r="C34" s="20"/>
       <c r="D34" s="14"/>
-      <c r="E34" s="15" t="e">
+      <c r="E34" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D34,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F34" s="16"/>
-      <c r="G34" s="17" t="e">
+      <c r="G34" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F34,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H34" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H34" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F34,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,18 +1497,24 @@
       <c r="B35" s="16"/>
       <c r="C35" s="20"/>
       <c r="D35" s="14"/>
-      <c r="E35" s="15" t="e">
+      <c r="E35" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D35,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F35" s="16"/>
-      <c r="G35" s="17" t="e">
+      <c r="G35" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F35,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H35" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H35" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F35,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,18 +1524,24 @@
       <c r="B36" s="16"/>
       <c r="C36" s="20"/>
       <c r="D36" s="14"/>
-      <c r="E36" s="15" t="e">
+      <c r="E36" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D36,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F36" s="16"/>
-      <c r="G36" s="17" t="e">
+      <c r="G36" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F36,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H36" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H36" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F36,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,18 +1551,24 @@
       <c r="B37" s="16"/>
       <c r="C37" s="20"/>
       <c r="D37" s="14"/>
-      <c r="E37" s="15" t="e">
+      <c r="E37" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D37,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F37" s="16"/>
-      <c r="G37" s="17" t="e">
+      <c r="G37" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F37,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H37" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H37" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F37,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,18 +1578,24 @@
       <c r="B38" s="16"/>
       <c r="C38" s="20"/>
       <c r="D38" s="14"/>
-      <c r="E38" s="15" t="e">
+      <c r="E38" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D38,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F38" s="16"/>
-      <c r="G38" s="17" t="e">
+      <c r="G38" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F38,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H38" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H38" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F38,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,18 +1605,24 @@
       <c r="B39" s="16"/>
       <c r="C39" s="20"/>
       <c r="D39" s="14"/>
-      <c r="E39" s="15" t="e">
+      <c r="E39" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D39,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F39" s="16"/>
-      <c r="G39" s="17" t="e">
+      <c r="G39" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F39,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H39" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H39" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F39,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,18 +1632,24 @@
       <c r="B40" s="16"/>
       <c r="C40" s="20"/>
       <c r="D40" s="14"/>
-      <c r="E40" s="15" t="e">
+      <c r="E40" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D40,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F40" s="16"/>
-      <c r="G40" s="17" t="e">
+      <c r="G40" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F40,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H40" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F40,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,18 +1659,24 @@
       <c r="B41" s="16"/>
       <c r="C41" s="20"/>
       <c r="D41" s="14"/>
-      <c r="E41" s="15" t="e">
+      <c r="E41" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D41,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F41" s="16"/>
-      <c r="G41" s="17" t="e">
+      <c r="G41" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F41,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H41" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H41" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F41,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,18 +1686,24 @@
       <c r="B42" s="16"/>
       <c r="C42" s="20"/>
       <c r="D42" s="14"/>
-      <c r="E42" s="15" t="e">
+      <c r="E42" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D42,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F42" s="16"/>
-      <c r="G42" s="17" t="e">
+      <c r="G42" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F42,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H42" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H42" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F42,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,18 +1713,24 @@
       <c r="B43" s="16"/>
       <c r="C43" s="20"/>
       <c r="D43" s="14"/>
-      <c r="E43" s="15" t="e">
+      <c r="E43" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D43,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F43" s="16"/>
-      <c r="G43" s="17" t="e">
+      <c r="G43" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F43,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H43" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H43" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F43,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,18 +1740,24 @@
       <c r="B44" s="16"/>
       <c r="C44" s="20"/>
       <c r="D44" s="14"/>
-      <c r="E44" s="15" t="e">
+      <c r="E44" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D44,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F44" s="16"/>
-      <c r="G44" s="17" t="e">
+      <c r="G44" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F44,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H44" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H44" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F44,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,18 +1767,24 @@
       <c r="B45" s="16"/>
       <c r="C45" s="20"/>
       <c r="D45" s="14"/>
-      <c r="E45" s="15" t="e">
+      <c r="E45" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D45,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F45" s="16"/>
-      <c r="G45" s="17" t="e">
+      <c r="G45" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F45,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H45" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H45" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F45,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,18 +1794,24 @@
       <c r="B46" s="16"/>
       <c r="C46" s="20"/>
       <c r="D46" s="14"/>
-      <c r="E46" s="15" t="e">
+      <c r="E46" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D46,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F46" s="16"/>
-      <c r="G46" s="17" t="e">
+      <c r="G46" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F46,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H46" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H46" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F46,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,18 +1821,24 @@
       <c r="B47" s="16"/>
       <c r="C47" s="20"/>
       <c r="D47" s="14"/>
-      <c r="E47" s="15" t="e">
+      <c r="E47" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D47,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F47" s="16"/>
-      <c r="G47" s="17" t="e">
+      <c r="G47" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F47,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H47" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H47" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F47,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,18 +1848,24 @@
       <c r="B48" s="16"/>
       <c r="C48" s="20"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="15" t="e">
+      <c r="E48" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D48,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F48" s="16"/>
-      <c r="G48" s="17" t="e">
+      <c r="G48" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F48,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H48" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H48" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F48,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,18 +1875,24 @@
       <c r="B49" s="16"/>
       <c r="C49" s="20"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="15" t="e">
+      <c r="E49" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D49,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F49" s="16"/>
-      <c r="G49" s="17" t="e">
+      <c r="G49" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F49,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H49" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H49" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F49,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,18 +1902,24 @@
       <c r="B50" s="16"/>
       <c r="C50" s="20"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="15" t="e">
+      <c r="E50" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D50,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F50" s="16"/>
-      <c r="G50" s="17" t="e">
+      <c r="G50" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F50,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H50" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H50" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F50,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,18 +1929,24 @@
       <c r="B51" s="16"/>
       <c r="C51" s="20"/>
       <c r="D51" s="14"/>
-      <c r="E51" s="15" t="e">
+      <c r="E51" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D51,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F51" s="16"/>
-      <c r="G51" s="17" t="e">
+      <c r="G51" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F51,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H51" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H51" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F51,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,18 +1956,24 @@
       <c r="B52" s="16"/>
       <c r="C52" s="20"/>
       <c r="D52" s="14"/>
-      <c r="E52" s="15" t="e">
+      <c r="E52" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D52,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F52" s="16"/>
-      <c r="G52" s="17" t="e">
+      <c r="G52" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F52,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H52" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H52" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F52,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,18 +1983,24 @@
       <c r="B53" s="16"/>
       <c r="C53" s="20"/>
       <c r="D53" s="14"/>
-      <c r="E53" s="15" t="e">
+      <c r="E53" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D53,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F53" s="16"/>
-      <c r="G53" s="17" t="e">
+      <c r="G53" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F53,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H53" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H53" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F53,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,18 +2010,24 @@
       <c r="B54" s="16"/>
       <c r="C54" s="20"/>
       <c r="D54" s="14"/>
-      <c r="E54" s="15" t="e">
+      <c r="E54" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D54,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F54" s="16"/>
-      <c r="G54" s="17" t="e">
+      <c r="G54" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F54,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H54" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H54" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F54,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,18 +2037,24 @@
       <c r="B55" s="16"/>
       <c r="C55" s="20"/>
       <c r="D55" s="14"/>
-      <c r="E55" s="15" t="e">
+      <c r="E55" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D55,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F55" s="16"/>
-      <c r="G55" s="17" t="e">
+      <c r="G55" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F55,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H55" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H55" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F55,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,18 +2064,24 @@
       <c r="B56" s="16"/>
       <c r="C56" s="20"/>
       <c r="D56" s="14"/>
-      <c r="E56" s="15" t="e">
+      <c r="E56" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D56,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F56" s="16"/>
-      <c r="G56" s="17" t="e">
+      <c r="G56" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F56,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H56" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H56" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F56,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,18 +2091,24 @@
       <c r="B57" s="16"/>
       <c r="C57" s="20"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="15" t="e">
+      <c r="E57" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D57,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F57" s="16"/>
-      <c r="G57" s="17" t="e">
+      <c r="G57" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F57,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H57" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H57" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F57,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,18 +2118,24 @@
       <c r="B58" s="16"/>
       <c r="C58" s="20"/>
       <c r="D58" s="14"/>
-      <c r="E58" s="15" t="e">
+      <c r="E58" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D58,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F58" s="16"/>
-      <c r="G58" s="17" t="e">
+      <c r="G58" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F58,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H58" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H58" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F58,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,18 +2145,24 @@
       <c r="B59" s="16"/>
       <c r="C59" s="20"/>
       <c r="D59" s="14"/>
-      <c r="E59" s="15" t="e">
+      <c r="E59" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D59,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F59" s="16"/>
-      <c r="G59" s="17" t="e">
+      <c r="G59" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F59,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H59" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H59" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F59,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,18 +2172,24 @@
       <c r="B60" s="16"/>
       <c r="C60" s="20"/>
       <c r="D60" s="14"/>
-      <c r="E60" s="15" t="e">
+      <c r="E60" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D60,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F60" s="16"/>
-      <c r="G60" s="17" t="e">
+      <c r="G60" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F60,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H60" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H60" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F60,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,18 +2199,24 @@
       <c r="B61" s="16"/>
       <c r="C61" s="20"/>
       <c r="D61" s="14"/>
-      <c r="E61" s="15" t="e">
+      <c r="E61" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D61,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F61" s="16"/>
-      <c r="G61" s="17" t="e">
+      <c r="G61" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F61,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H61" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H61" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F61,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,18 +2226,24 @@
       <c r="B62" s="16"/>
       <c r="C62" s="20"/>
       <c r="D62" s="14"/>
-      <c r="E62" s="15" t="e">
+      <c r="E62" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D62,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F62" s="16"/>
-      <c r="G62" s="17" t="e">
+      <c r="G62" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F62,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H62" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H62" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F62,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,18 +2253,24 @@
       <c r="B63" s="16"/>
       <c r="C63" s="20"/>
       <c r="D63" s="14"/>
-      <c r="E63" s="15" t="e">
+      <c r="E63" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D63,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F63" s="16"/>
-      <c r="G63" s="17" t="e">
+      <c r="G63" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F63,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H63" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H63" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F63,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,18 +2280,24 @@
       <c r="B64" s="16"/>
       <c r="C64" s="20"/>
       <c r="D64" s="14"/>
-      <c r="E64" s="15" t="e">
+      <c r="E64" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D64,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F64" s="16"/>
-      <c r="G64" s="17" t="e">
+      <c r="G64" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F64,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H64" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H64" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F64,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,18 +2307,24 @@
       <c r="B65" s="16"/>
       <c r="C65" s="20"/>
       <c r="D65" s="14"/>
-      <c r="E65" s="15" t="e">
+      <c r="E65" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D65,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F65" s="16"/>
-      <c r="G65" s="17" t="e">
+      <c r="G65" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F65,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H65" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H65" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F65,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,18 +2334,24 @@
       <c r="B66" s="16"/>
       <c r="C66" s="20"/>
       <c r="D66" s="14"/>
-      <c r="E66" s="15" t="e">
+      <c r="E66" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D66,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F66" s="16"/>
-      <c r="G66" s="17" t="e">
+      <c r="G66" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F66,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H66" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H66" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F66,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,18 +2361,24 @@
       <c r="B67" s="16"/>
       <c r="C67" s="20"/>
       <c r="D67" s="14"/>
-      <c r="E67" s="15" t="e">
+      <c r="E67" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D67,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F67" s="16"/>
-      <c r="G67" s="17" t="e">
+      <c r="G67" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F67,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H67" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H67" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F67,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,18 +2388,24 @@
       <c r="B68" s="16"/>
       <c r="C68" s="20"/>
       <c r="D68" s="14"/>
-      <c r="E68" s="15" t="e">
+      <c r="E68" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D68,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F68" s="16"/>
-      <c r="G68" s="17" t="e">
+      <c r="G68" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F68,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H68" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H68" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F68,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,18 +2415,24 @@
       <c r="B69" s="16"/>
       <c r="C69" s="20"/>
       <c r="D69" s="14"/>
-      <c r="E69" s="15" t="e">
+      <c r="E69" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D69,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F69" s="16"/>
-      <c r="G69" s="17" t="e">
+      <c r="G69" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F69,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H69" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H69" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F69,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,18 +2442,24 @@
       <c r="B70" s="16"/>
       <c r="C70" s="20"/>
       <c r="D70" s="14"/>
-      <c r="E70" s="15" t="e">
+      <c r="E70" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D70,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F70" s="16"/>
-      <c r="G70" s="17" t="e">
+      <c r="G70" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F70,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H70" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H70" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F70,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,18 +2469,24 @@
       <c r="B71" s="16"/>
       <c r="C71" s="20"/>
       <c r="D71" s="14"/>
-      <c r="E71" s="15" t="e">
+      <c r="E71" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D71,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F71" s="16"/>
-      <c r="G71" s="17" t="e">
+      <c r="G71" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F71,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H71" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H71" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F71,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,18 +2496,24 @@
       <c r="B72" s="16"/>
       <c r="C72" s="20"/>
       <c r="D72" s="14"/>
-      <c r="E72" s="15" t="e">
+      <c r="E72" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D72,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F72" s="16"/>
-      <c r="G72" s="17" t="e">
+      <c r="G72" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F72,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H72" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H72" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F72,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,18 +2523,24 @@
       <c r="B73" s="16"/>
       <c r="C73" s="20"/>
       <c r="D73" s="14"/>
-      <c r="E73" s="15" t="e">
+      <c r="E73" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D73,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F73" s="16"/>
-      <c r="G73" s="17" t="e">
+      <c r="G73" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F73,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H73" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H73" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F73,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,18 +2550,24 @@
       <c r="B74" s="16"/>
       <c r="C74" s="20"/>
       <c r="D74" s="14"/>
-      <c r="E74" s="15" t="e">
+      <c r="E74" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D74,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F74" s="16"/>
-      <c r="G74" s="17" t="e">
+      <c r="G74" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F74,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H74" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H74" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F74,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,18 +2577,24 @@
       <c r="B75" s="16"/>
       <c r="C75" s="20"/>
       <c r="D75" s="14"/>
-      <c r="E75" s="15" t="e">
+      <c r="E75" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D75,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F75" s="16"/>
-      <c r="G75" s="17" t="e">
+      <c r="G75" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F75,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H75" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H75" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F75,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,18 +2604,24 @@
       <c r="B76" s="16"/>
       <c r="C76" s="20"/>
       <c r="D76" s="14"/>
-      <c r="E76" s="15" t="e">
+      <c r="E76" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D76,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F76" s="16"/>
-      <c r="G76" s="17" t="e">
+      <c r="G76" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F76,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H76" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H76" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F76,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,18 +2631,24 @@
       <c r="B77" s="16"/>
       <c r="C77" s="20"/>
       <c r="D77" s="14"/>
-      <c r="E77" s="15" t="e">
+      <c r="E77" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D77,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F77" s="16"/>
-      <c r="G77" s="17" t="e">
+      <c r="G77" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F77,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H77" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H77" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F77,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,18 +2658,24 @@
       <c r="B78" s="16"/>
       <c r="C78" s="20"/>
       <c r="D78" s="14"/>
-      <c r="E78" s="15" t="e">
+      <c r="E78" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D78,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F78" s="16"/>
-      <c r="G78" s="17" t="e">
+      <c r="G78" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F78,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H78" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H78" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F78,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,18 +2685,24 @@
       <c r="B79" s="16"/>
       <c r="C79" s="20"/>
       <c r="D79" s="14"/>
-      <c r="E79" s="15" t="e">
+      <c r="E79" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D79,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F79" s="16"/>
-      <c r="G79" s="17" t="e">
+      <c r="G79" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F79,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H79" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H79" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F79,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,18 +2712,24 @@
       <c r="B80" s="16"/>
       <c r="C80" s="20"/>
       <c r="D80" s="14"/>
-      <c r="E80" s="15" t="e">
+      <c r="E80" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D80,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F80" s="16"/>
-      <c r="G80" s="17" t="e">
+      <c r="G80" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F80,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H80" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H80" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F80,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,18 +2739,24 @@
       <c r="B81" s="16"/>
       <c r="C81" s="20"/>
       <c r="D81" s="14"/>
-      <c r="E81" s="15" t="e">
+      <c r="E81" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D81,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F81" s="16"/>
-      <c r="G81" s="17" t="e">
+      <c r="G81" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F81,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H81" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H81" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F81,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,18 +2766,24 @@
       <c r="B82" s="16"/>
       <c r="C82" s="20"/>
       <c r="D82" s="14"/>
-      <c r="E82" s="15" t="e">
+      <c r="E82" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D82,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F82" s="16"/>
-      <c r="G82" s="17" t="e">
+      <c r="G82" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F82,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H82" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H82" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F82,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,18 +2793,24 @@
       <c r="B83" s="16"/>
       <c r="C83" s="20"/>
       <c r="D83" s="14"/>
-      <c r="E83" s="15" t="e">
+      <c r="E83" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D83,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F83" s="16"/>
-      <c r="G83" s="17" t="e">
+      <c r="G83" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F83,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H83" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H83" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F83,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,18 +2820,24 @@
       <c r="B84" s="16"/>
       <c r="C84" s="20"/>
       <c r="D84" s="14"/>
-      <c r="E84" s="15" t="e">
+      <c r="E84" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D84,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F84" s="16"/>
-      <c r="G84" s="17" t="e">
+      <c r="G84" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F84,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H84" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H84" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F84,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,18 +2847,24 @@
       <c r="B85" s="16"/>
       <c r="C85" s="20"/>
       <c r="D85" s="14"/>
-      <c r="E85" s="15" t="e">
+      <c r="E85" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D85,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F85" s="16"/>
-      <c r="G85" s="17" t="e">
+      <c r="G85" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F85,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H85" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H85" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F85,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,18 +2874,24 @@
       <c r="B86" s="16"/>
       <c r="C86" s="20"/>
       <c r="D86" s="14"/>
-      <c r="E86" s="15" t="e">
+      <c r="E86" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D86,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F86" s="16"/>
-      <c r="G86" s="17" t="e">
+      <c r="G86" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F86,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H86" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H86" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F86,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2406,18 +2901,24 @@
       <c r="B87" s="16"/>
       <c r="C87" s="20"/>
       <c r="D87" s="14"/>
-      <c r="E87" s="15" t="e">
+      <c r="E87" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D87,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F87" s="16"/>
-      <c r="G87" s="17" t="e">
+      <c r="G87" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F87,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H87" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H87" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F87,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,18 +2928,24 @@
       <c r="B88" s="16"/>
       <c r="C88" s="20"/>
       <c r="D88" s="14"/>
-      <c r="E88" s="15" t="e">
+      <c r="E88" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D88,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F88" s="16"/>
-      <c r="G88" s="17" t="e">
+      <c r="G88" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F88,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H88" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H88" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F88,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,18 +2955,24 @@
       <c r="B89" s="16"/>
       <c r="C89" s="20"/>
       <c r="D89" s="14"/>
-      <c r="E89" s="15" t="e">
+      <c r="E89" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D89,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F89" s="16"/>
-      <c r="G89" s="17" t="e">
+      <c r="G89" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F89,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H89" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H89" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F89,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,18 +2982,24 @@
       <c r="B90" s="16"/>
       <c r="C90" s="20"/>
       <c r="D90" s="14"/>
-      <c r="E90" s="15" t="e">
+      <c r="E90" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D90,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F90" s="16"/>
-      <c r="G90" s="17" t="e">
+      <c r="G90" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F90,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H90" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H90" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F90,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,18 +3009,24 @@
       <c r="B91" s="16"/>
       <c r="C91" s="20"/>
       <c r="D91" s="14"/>
-      <c r="E91" s="15" t="e">
+      <c r="E91" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D91,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F91" s="16"/>
-      <c r="G91" s="17" t="e">
+      <c r="G91" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F91,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H91" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H91" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F91,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,18 +3036,24 @@
       <c r="B92" s="16"/>
       <c r="C92" s="20"/>
       <c r="D92" s="14"/>
-      <c r="E92" s="15" t="e">
+      <c r="E92" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D92,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F92" s="16"/>
-      <c r="G92" s="17" t="e">
+      <c r="G92" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F92,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H92" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H92" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F92,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,18 +3063,24 @@
       <c r="B93" s="16"/>
       <c r="C93" s="20"/>
       <c r="D93" s="14"/>
-      <c r="E93" s="15" t="e">
+      <c r="E93" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D93,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F93" s="16"/>
-      <c r="G93" s="17" t="e">
+      <c r="G93" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F93,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H93" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H93" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F93,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,18 +3090,24 @@
       <c r="B94" s="16"/>
       <c r="C94" s="20"/>
       <c r="D94" s="14"/>
-      <c r="E94" s="15" t="e">
+      <c r="E94" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D94,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F94" s="16"/>
-      <c r="G94" s="17" t="e">
+      <c r="G94" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F94,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H94" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H94" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F94,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,18 +3117,24 @@
       <c r="B95" s="16"/>
       <c r="C95" s="20"/>
       <c r="D95" s="14"/>
-      <c r="E95" s="15" t="e">
+      <c r="E95" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D95,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F95" s="16"/>
-      <c r="G95" s="17" t="e">
+      <c r="G95" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F95,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H95" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H95" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F95,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,18 +3144,24 @@
       <c r="B96" s="16"/>
       <c r="C96" s="20"/>
       <c r="D96" s="14"/>
-      <c r="E96" s="15" t="e">
+      <c r="E96" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D96,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F96" s="16"/>
-      <c r="G96" s="17" t="e">
+      <c r="G96" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F96,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H96" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H96" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F96,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,18 +3171,24 @@
       <c r="B97" s="16"/>
       <c r="C97" s="20"/>
       <c r="D97" s="14"/>
-      <c r="E97" s="15" t="e">
+      <c r="E97" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D97,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F97" s="16"/>
-      <c r="G97" s="17" t="e">
+      <c r="G97" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F97,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H97" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H97" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F97,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,18 +3198,24 @@
       <c r="B98" s="16"/>
       <c r="C98" s="20"/>
       <c r="D98" s="14"/>
-      <c r="E98" s="15" t="e">
+      <c r="E98" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D98,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F98" s="16"/>
-      <c r="G98" s="17" t="e">
+      <c r="G98" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F98,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H98" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H98" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F98,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,18 +3225,24 @@
       <c r="B99" s="16"/>
       <c r="C99" s="20"/>
       <c r="D99" s="14"/>
-      <c r="E99" s="15" t="e">
+      <c r="E99" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D99,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F99" s="16"/>
-      <c r="G99" s="17" t="e">
+      <c r="G99" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F99,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H99" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H99" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F99,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,18 +3252,24 @@
       <c r="B100" s="16"/>
       <c r="C100" s="20"/>
       <c r="D100" s="14"/>
-      <c r="E100" s="15" t="e">
+      <c r="E100" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D100,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F100" s="16"/>
-      <c r="G100" s="17" t="e">
+      <c r="G100" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F100,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H100" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H100" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F100,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,18 +3279,24 @@
       <c r="B101" s="16"/>
       <c r="C101" s="20"/>
       <c r="D101" s="14"/>
-      <c r="E101" s="15" t="e">
+      <c r="E101" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D101,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F101" s="16"/>
-      <c r="G101" s="17" t="e">
+      <c r="G101" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F101,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H101" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H101" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F101,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,18 +3306,24 @@
       <c r="B102" s="16"/>
       <c r="C102" s="20"/>
       <c r="D102" s="14"/>
-      <c r="E102" s="15" t="e">
+      <c r="E102" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D102,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F102" s="16"/>
-      <c r="G102" s="17" t="e">
+      <c r="G102" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F102,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H102" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H102" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F102,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,27 +3333,33 @@
       <c r="B103" s="16"/>
       <c r="C103" s="20"/>
       <c r="D103" s="14"/>
-      <c r="E103" s="15" t="e">
+      <c r="E103" s="15" t="inlineStr">
         <f aca="false">VLOOKUP(D103,$J$23:$K$26,2)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F103" s="16"/>
-      <c r="G103" s="17" t="e">
+      <c r="G103" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F103,$J$4:$L$19,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H103" s="17" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H103" s="17" t="inlineStr">
         <f aca="false">VLOOKUP(F103,$J$4:$L$19,3)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="23"/>
       <c r="B104" s="23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D104" s="23"/>
       <c r="E104" s="25"/>

</xml_diff>